<commit_message>
added NGC1818 ROB D1 to target tables
</commit_message>
<xml_diff>
--- a/data/target_metadata/LMC_SMC_sample.xlsx
+++ b/data/target_metadata/LMC_SMC_sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duval/Documents/ULLYSES/TARGET_SELECTION/MASSIVE_STARS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/user/duval/ULLYSES/ullyses_tech/jira_connection/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056FCCA2-D39E-A244-B6E7-78A44C7B6407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07DCBB1-44DA-3342-86A0-3C097BB7456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="860" windowWidth="29220" windowHeight="16240" xr2:uid="{B63D01DA-0498-B443-A193-19112F8FC86D}"/>
+    <workbookView xWindow="2640" yWindow="460" windowWidth="35740" windowHeight="18660" xr2:uid="{B63D01DA-0498-B443-A193-19112F8FC86D}"/>
   </bookViews>
   <sheets>
     <sheet name="LMC" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3125" uniqueCount="1733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3135" uniqueCount="1739">
   <si>
     <t>Target</t>
   </si>
@@ -5232,6 +5232,24 @@
   </si>
   <si>
     <t>ACTUAl ORBS</t>
+  </si>
+  <si>
+    <t>NGC1818 ROB D1</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://simbad.u-strasbg.fr/simbad/sim-id?Ident=Cl*+NGC+1818+ROB+D1&amp;submit=submit+id" target="_blank"&gt; NGC1818 ROB D1&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>05h04m32.31s</t>
+  </si>
+  <si>
+    <t>-66d24m47.57</t>
+  </si>
+  <si>
+    <t>B1.5V</t>
+  </si>
+  <si>
+    <t>COS/G130M/1291-1327-COS/G160M/1577-1623-COS/G185M/1913-1941-1971-2010-COS/G225M-2233-2268-2306</t>
   </si>
 </sst>
 </file>
@@ -5363,7 +5381,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -5371,6 +5389,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -5692,9 +5711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C815C55B-6D46-094D-9AD8-F2F59E8E22E1}">
   <dimension ref="A1:AL153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N163" sqref="N163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18343,25 +18362,75 @@
       </c>
     </row>
     <row r="153" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="Q153">
-        <f>SUM(Q2:Q152)</f>
-        <v>231</v>
-      </c>
-      <c r="R153">
-        <f>SUM(R2:R152)</f>
-        <v>237</v>
-      </c>
-      <c r="U153">
-        <f>SUM(U2:U152)</f>
-        <v>120</v>
-      </c>
-      <c r="V153">
-        <f>SUM(V2:V152)</f>
-        <v>104</v>
-      </c>
-      <c r="W153">
-        <f>SUM(W2:W152)</f>
-        <v>111</v>
+      <c r="A153" s="1" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D153" s="7" t="s">
+        <v>1736</v>
+      </c>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+      <c r="I153" s="1"/>
+      <c r="J153" s="1" t="s">
+        <v>1737</v>
+      </c>
+      <c r="K153" s="1"/>
+      <c r="L153" s="1"/>
+      <c r="M153" s="1"/>
+      <c r="N153" s="1"/>
+      <c r="O153" s="1">
+        <v>0</v>
+      </c>
+      <c r="P153" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q153" s="1">
+        <v>0</v>
+      </c>
+      <c r="R153" s="1">
+        <v>0</v>
+      </c>
+      <c r="S153" s="1"/>
+      <c r="T153" s="1"/>
+      <c r="U153" s="1"/>
+      <c r="V153" s="1"/>
+      <c r="W153" s="1"/>
+      <c r="X153" s="1"/>
+      <c r="Y153" s="1"/>
+      <c r="Z153" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AA153" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB153" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC153" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD153" s="1"/>
+      <c r="AE153" s="1"/>
+      <c r="AF153" s="1"/>
+      <c r="AG153" s="1"/>
+      <c r="AH153" s="1" t="s">
+        <v>1738</v>
+      </c>
+      <c r="AI153" s="1"/>
+      <c r="AJ153" s="1"/>
+      <c r="AK153" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL153" s="1">
+        <v>14081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>